<commit_message>
update color in dataflow chart
</commit_message>
<xml_diff>
--- a/data/topology-entry.xlsx
+++ b/data/topology-entry.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guannanzhou/Desktop/工作/09.解决方案/03.adhoc/06.AI/topology/topology_app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A86D43A-F8BB-0E44-953F-9EE594C8375A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0484C136-F456-284B-9553-50BD4300064E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16780" activeTab="1" xr2:uid="{1B9DFEE4-4773-DF4C-9923-82383A3D4CAA}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16640" activeTab="1" xr2:uid="{1B9DFEE4-4773-DF4C-9923-82383A3D4CAA}"/>
   </bookViews>
   <sheets>
     <sheet name="Interface" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="122">
   <si>
     <t>No</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -440,10 +440,6 @@
   </si>
   <si>
     <t>文件样本</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>下发策略</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -895,7 +891,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C2" t="s">
         <v>90</v>
@@ -979,7 +975,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C9" t="s">
         <v>90</v>
@@ -991,7 +987,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C10" t="s">
         <v>90</v>
@@ -1003,7 +999,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C11" t="s">
         <v>90</v>
@@ -1163,8 +1159,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F360BAF8-4A8A-4D40-B70E-A17CF1A4D8E5}">
   <dimension ref="A1:AI33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="90" workbookViewId="0">
+      <selection activeCell="O26" sqref="O26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1200,7 +1196,7 @@
         <v>3</v>
       </c>
       <c r="I1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J1" t="s">
         <v>55</v>
@@ -1373,7 +1369,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C4" t="s">
         <v>19</v>
@@ -1475,7 +1471,7 @@
         <v>37</v>
       </c>
       <c r="I8" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="K8" t="s">
         <v>104</v>
@@ -1751,7 +1747,7 @@
         <v>95</v>
       </c>
       <c r="AF20" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="21" spans="1:32">
@@ -1766,7 +1762,7 @@
         <v>11</v>
       </c>
       <c r="Z21" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="22" spans="1:32">
@@ -1784,7 +1780,7 @@
         <v>10</v>
       </c>
       <c r="Z22" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="23" spans="1:32">
@@ -1931,7 +1927,7 @@
         <v>104</v>
       </c>
       <c r="M28" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="29" spans="1:32">
@@ -1999,7 +1995,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C13"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>